<commit_message>
chore(i18n): normalize PT-BR accents (UTF-8) in UI labels and responses\n\n- Infrastructure, SketchSection, RulesSection, BasicInfo, Documentation\n- Ensure Flask JSON responses are UTF-8 (JSON_AS_ASCII=False) and NFC normalization
</commit_message>
<xml_diff>
--- a/Planilha_Visita_Site.xlsx
+++ b/Planilha_Visita_Site.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trabalhos em python\aplicativo_relatorio_de_visita_externa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB51846-7B9E-40E9-B27A-B7259F02DC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64ED5B07-FEF4-49CA-AD7C-5E4E6D556EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informações do Site" sheetId="1" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1742,18 +1742,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.85546875" customWidth="1"/>
-    <col min="3" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="78.5703125" customWidth="1"/>
-    <col min="6" max="10" width="27.42578125" customWidth="1"/>
+    <col min="1" max="10" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>